<commit_message>
Estudo da velocidade e aceleração dos dados
</commit_message>
<xml_diff>
--- a/data_analysis_google_sheets/clube_do_livro.xlsx
+++ b/data_analysis_google_sheets/clube_do_livro.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="35">
   <si>
     <t>LIVROS</t>
   </si>
@@ -111,6 +111,12 @@
   </si>
   <si>
     <t>Vendas</t>
+  </si>
+  <si>
+    <t>Velocidade</t>
+  </si>
+  <si>
+    <t>Aceleração</t>
   </si>
 </sst>
 </file>
@@ -120,7 +126,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[$R$ -416]#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="9">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -162,8 +168,19 @@
       <color rgb="FF000000"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -188,6 +205,12 @@
         <bgColor rgb="FF0000FF"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC9DAF8"/>
+        <bgColor rgb="FFC9DAF8"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border/>
@@ -209,7 +232,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -237,15 +260,18 @@
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf borderId="0" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFill="1" applyFont="1">
+    <xf borderId="1" fillId="4" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFill="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
+    <xf borderId="1" fillId="0" fontId="6" numFmtId="164" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1" applyNumberFormat="1">
       <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="0" xfId="0" applyBorder="1" applyFont="1"/>
+    <xf borderId="1" fillId="0" fontId="7" numFmtId="164" xfId="0" applyBorder="1" applyFont="1" applyNumberFormat="1"/>
+    <xf borderId="1" fillId="5" fontId="8" numFmtId="164" xfId="0" applyBorder="1" applyFill="1" applyFont="1" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle xfId="0" name="Normal" builtinId="0"/>
@@ -362,11 +388,11 @@
             </c:numRef>
           </c:val>
         </c:ser>
-        <c:axId val="941674743"/>
-        <c:axId val="1126471046"/>
+        <c:axId val="534819919"/>
+        <c:axId val="1685723138"/>
       </c:bar3DChart>
       <c:catAx>
-        <c:axId val="941674743"/>
+        <c:axId val="534819919"/>
         <c:scaling>
           <c:orientation val="maxMin"/>
         </c:scaling>
@@ -418,10 +444,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1126471046"/>
+        <c:crossAx val="1685723138"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1126471046"/>
+        <c:axId val="1685723138"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -498,7 +524,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="941674743"/>
+        <c:crossAx val="534819919"/>
         <c:crosses val="max"/>
       </c:valAx>
     </c:plotArea>
@@ -540,17 +566,17 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr lvl="0">
-              <a:defRPr b="0">
+              <a:defRPr b="1">
                 <a:solidFill>
-                  <a:srgbClr val="757575"/>
+                  <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr b="0">
+              <a:rPr b="1">
                 <a:solidFill>
-                  <a:srgbClr val="757575"/>
+                  <a:srgbClr val="000000"/>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
               </a:rPr>
@@ -611,11 +637,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1796748489"/>
-        <c:axId val="1215183499"/>
+        <c:axId val="867786064"/>
+        <c:axId val="2044145723"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1796748489"/>
+        <c:axId val="867786064"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -667,10 +693,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1215183499"/>
+        <c:crossAx val="2044145723"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1215183499"/>
+        <c:axId val="2044145723"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -745,7 +771,512 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1796748489"/>
+        <c:crossAx val="867786064"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="1A1A1A"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="1">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Velocidade de vendas por semana</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página02'!$C$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng">
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="4285F4"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:name>Linha de tendência para Velocidade</c:name>
+            <c:spPr>
+              <a:ln w="38100">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000">
+                    <a:alpha val="60000"/>
+                  </a:srgbClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página02'!$A$2:$A$15</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página02'!$C$2:$C$15</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="1770490580"/>
+        <c:axId val="2136414752"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1770490580"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Semanas</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2136414752"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2136414752"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t>Velocidade</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1770490580"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:txPr>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr lvl="0">
+            <a:defRPr b="0">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+            </a:defRPr>
+          </a:pPr>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+  </c:chart>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:mv="urn:schemas-microsoft-com:mac:vml" xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart">
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="1">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr b="1">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
+              <a:t>Aceleração do valor de vendas</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Página02'!$D$1</c:f>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln cmpd="sng" w="19050">
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+              <a:prstDash val="solid"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="4285F4"/>
+              </a:solidFill>
+              <a:ln cmpd="sng">
+                <a:solidFill>
+                  <a:srgbClr val="4285F4"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:name>Linha de tendência para Aceleração</c:name>
+            <c:spPr>
+              <a:ln w="38100">
+                <a:solidFill>
+                  <a:srgbClr val="FF0000">
+                    <a:alpha val="70196"/>
+                  </a:srgbClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="0"/>
+          </c:trendline>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Página02'!$A$2:$A$15</c:f>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Página02'!$D$2:$D$15</c:f>
+              <c:numCache/>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:axId val="1442755178"/>
+        <c:axId val="2211208"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1442755178"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:spPr/>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2211208"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2211208"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="B7B7B7"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:srgbClr val="CCCCCC">
+                  <a:alpha val="0"/>
+                </a:srgbClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr lvl="0">
+                  <a:defRPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr b="0">
+                    <a:solidFill>
+                      <a:srgbClr val="000000"/>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
+                  <a:t/>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:ln/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr lvl="0">
+              <a:defRPr b="0">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+              </a:defRPr>
+            </a:pPr>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1442755178"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -805,12 +1336,12 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:cx="http://schemas.microsoft.com/office/drawing/2014/chartex" xmlns:cx1="http://schemas.microsoft.com/office/drawing/2015/9/8/chartex" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:x3Unk="http://schemas.microsoft.com/office/drawing/2010/slicer" xmlns:sle15="http://schemas.microsoft.com/office/drawing/2012/slicer">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>1</xdr:col>
-      <xdr:colOff>1104900</xdr:colOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>933450</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5715000" cy="3533775"/>
+    <xdr:ext cx="4991100" cy="4581525"/>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 2" title="Gráfico"/>
@@ -823,6 +1354,56 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4781550" cy="2314575"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 3" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>952500</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>133350</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="4781550" cy="2266950"/>
+    <xdr:graphicFrame>
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 4" title="Gráfico"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1443,6 +2024,12 @@
       <c r="B1" s="9" t="s">
         <v>32</v>
       </c>
+      <c r="C1" s="9" t="s">
+        <v>33</v>
+      </c>
+      <c r="D1" s="9" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="2">
       <c r="A2" s="10">
@@ -1451,6 +2038,8 @@
       <c r="B2" s="11">
         <v>800.0</v>
       </c>
+      <c r="C2" s="12"/>
+      <c r="D2" s="12"/>
     </row>
     <row r="3">
       <c r="A3" s="10">
@@ -1459,6 +2048,11 @@
       <c r="B3" s="11">
         <v>640.0</v>
       </c>
+      <c r="C3" s="13">
+        <f t="shared" ref="C3:C15" si="1">B3-B2</f>
+        <v>-160</v>
+      </c>
+      <c r="D3" s="12"/>
     </row>
     <row r="4">
       <c r="A4" s="10">
@@ -1467,6 +2061,14 @@
       <c r="B4" s="11">
         <v>800.0</v>
       </c>
+      <c r="C4" s="13">
+        <f t="shared" si="1"/>
+        <v>160</v>
+      </c>
+      <c r="D4" s="13">
+        <f t="shared" ref="D4:D15" si="2">C4-C3</f>
+        <v>320</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" s="10">
@@ -1475,6 +2077,14 @@
       <c r="B5" s="11">
         <v>700.0</v>
       </c>
+      <c r="C5" s="13">
+        <f t="shared" si="1"/>
+        <v>-100</v>
+      </c>
+      <c r="D5" s="13">
+        <f t="shared" si="2"/>
+        <v>-260</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" s="10">
@@ -1483,6 +2093,14 @@
       <c r="B6" s="11">
         <v>930.0</v>
       </c>
+      <c r="C6" s="13">
+        <f t="shared" si="1"/>
+        <v>230</v>
+      </c>
+      <c r="D6" s="13">
+        <f t="shared" si="2"/>
+        <v>330</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" s="10">
@@ -1491,6 +2109,14 @@
       <c r="B7" s="11">
         <v>1120.0</v>
       </c>
+      <c r="C7" s="13">
+        <f t="shared" si="1"/>
+        <v>190</v>
+      </c>
+      <c r="D7" s="13">
+        <f t="shared" si="2"/>
+        <v>-40</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" s="10">
@@ -1499,6 +2125,14 @@
       <c r="B8" s="11">
         <v>945.0</v>
       </c>
+      <c r="C8" s="13">
+        <f t="shared" si="1"/>
+        <v>-175</v>
+      </c>
+      <c r="D8" s="13">
+        <f t="shared" si="2"/>
+        <v>-365</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" s="10">
@@ -1507,6 +2141,14 @@
       <c r="B9" s="11">
         <v>900.0</v>
       </c>
+      <c r="C9" s="13">
+        <f t="shared" si="1"/>
+        <v>-45</v>
+      </c>
+      <c r="D9" s="13">
+        <f t="shared" si="2"/>
+        <v>130</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" s="10">
@@ -1515,6 +2157,14 @@
       <c r="B10" s="11">
         <v>1200.0</v>
       </c>
+      <c r="C10" s="13">
+        <f t="shared" si="1"/>
+        <v>300</v>
+      </c>
+      <c r="D10" s="13">
+        <f t="shared" si="2"/>
+        <v>345</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" s="10">
@@ -1523,6 +2173,14 @@
       <c r="B11" s="11">
         <v>1300.0</v>
       </c>
+      <c r="C11" s="13">
+        <f t="shared" si="1"/>
+        <v>100</v>
+      </c>
+      <c r="D11" s="13">
+        <f t="shared" si="2"/>
+        <v>-200</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="10">
@@ -1531,6 +2189,14 @@
       <c r="B12" s="11">
         <v>1100.0</v>
       </c>
+      <c r="C12" s="13">
+        <f t="shared" si="1"/>
+        <v>-200</v>
+      </c>
+      <c r="D12" s="13">
+        <f t="shared" si="2"/>
+        <v>-300</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" s="10">
@@ -1539,6 +2205,14 @@
       <c r="B13" s="11">
         <v>1100.0</v>
       </c>
+      <c r="C13" s="13">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="D13" s="13">
+        <f t="shared" si="2"/>
+        <v>200</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" s="10">
@@ -1547,6 +2221,14 @@
       <c r="B14" s="11">
         <v>900.0</v>
       </c>
+      <c r="C14" s="13">
+        <f t="shared" si="1"/>
+        <v>-200</v>
+      </c>
+      <c r="D14" s="13">
+        <f t="shared" si="2"/>
+        <v>-200</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" s="10">
@@ -1554,6 +2236,31 @@
       </c>
       <c r="B15" s="11">
         <v>930.0</v>
+      </c>
+      <c r="C15" s="13">
+        <f t="shared" si="1"/>
+        <v>30</v>
+      </c>
+      <c r="D15" s="13">
+        <f t="shared" si="2"/>
+        <v>230</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16" s="14">
+        <f>SUM(B2:B15)</f>
+        <v>13365</v>
+      </c>
+      <c r="C16" s="14">
+        <f>SUM(C3:C15)</f>
+        <v>130</v>
+      </c>
+      <c r="D16" s="14">
+        <f>SUM(D4:D15)</f>
+        <v>190</v>
       </c>
     </row>
   </sheetData>

</xml_diff>